<commit_message>
"Changed the test runner path for features"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -283,6 +283,45 @@
   </si>
   <si>
     <t>42 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. Ramesh D</t>
+  </si>
+  <si>
+    <t>31 years experience overall</t>
+  </si>
+  <si>
+    <t>Ashok Nagar,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Vikram P S J</t>
+  </si>
+  <si>
+    <t>Greams Road,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Balaji R</t>
+  </si>
+  <si>
+    <t>24 years experience overall</t>
+  </si>
+  <si>
+    <t>Thousand Lights,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Nitya Narayanan</t>
+  </si>
+  <si>
+    <t>29 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. Sudha Anantha Krishnan</t>
+  </si>
+  <si>
+    <t>27 years experience overall</t>
+  </si>
+  <si>
+    <t>Kilpauk,Chennai</t>
   </si>
 </sst>
 </file>
@@ -790,16 +829,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -807,16 +846,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -824,16 +863,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -841,16 +880,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -858,16 +897,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"Added excel wb and assert checked for surgeries"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2318520\eclipse-workspace\hackathon2\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2318520\eclipse-workspace\Hackathon_Practo\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C528FA8-60A7-4A1A-B6CF-FE1E36AF854A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFC8F1C-F0D7-4986-B6DB-7A6CD7F0EDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="708" windowWidth="23040" windowHeight="11532" activeTab="1" xr2:uid="{CCA4E1CD-FF9D-4CD4-B2D1-E3BACCC0835E}"/>
+    <workbookView xWindow="0" yWindow="708" windowWidth="23040" windowHeight="11532" xr2:uid="{CCA4E1CD-FF9D-4CD4-B2D1-E3BACCC0835E}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -159,169 +159,97 @@
     <t>john_cena@gmail.com</t>
   </si>
   <si>
-    <t>Dr. Rikin Gogri</t>
-  </si>
-  <si>
-    <t>Dentist</t>
-  </si>
-  <si>
-    <t>23 years experience overall</t>
-  </si>
-  <si>
-    <t>Goregaon West,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Aashiq Shaikh</t>
-  </si>
-  <si>
-    <t>15 years experience overall</t>
-  </si>
-  <si>
-    <t>Bhandup West,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Nitesh Motwani</t>
-  </si>
-  <si>
-    <t>16 years experience overall</t>
-  </si>
-  <si>
-    <t>Andheri West,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Upasana Gosalia</t>
-  </si>
-  <si>
-    <t>Ghatkopar East,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Vivian Varghese</t>
-  </si>
-  <si>
     <t>13 years experience overall</t>
   </si>
   <si>
-    <t>Borivali West,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Shivprakash Mehta</t>
-  </si>
-  <si>
     <t>Ear-Nose-Throat (ENT) Specialist</t>
   </si>
   <si>
-    <t>Sadashiv Peth,Pune</t>
-  </si>
-  <si>
-    <t>Dr. Rupalee Borkar</t>
-  </si>
-  <si>
-    <t>9 years experience overall</t>
-  </si>
-  <si>
-    <t>Kharadi,Pune</t>
-  </si>
-  <si>
-    <t>Dr. Shalini Saxena</t>
-  </si>
-  <si>
-    <t>26 years experience overall</t>
-  </si>
-  <si>
-    <t>Pimpri-Chinchwad,Pune</t>
-  </si>
-  <si>
-    <t>Dr. Devayani B Shinde</t>
-  </si>
-  <si>
-    <t>Kalyani Nagar,Pune</t>
-  </si>
-  <si>
-    <t>Dr. Priyanka Aage</t>
-  </si>
-  <si>
-    <t>10 years experience overall</t>
-  </si>
-  <si>
-    <t>Aundh,Pune</t>
-  </si>
-  <si>
-    <t>Dr. Vivek Pal Singh</t>
-  </si>
-  <si>
-    <t>Internal Medicine</t>
-  </si>
-  <si>
-    <t>19 years experience overall</t>
-  </si>
-  <si>
-    <t>Pusa Road,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Manoj Ranka</t>
-  </si>
-  <si>
-    <t>21 years experience overall</t>
-  </si>
-  <si>
-    <t>Saket,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Anil Vardani</t>
-  </si>
-  <si>
-    <t>38 years experience overall</t>
-  </si>
-  <si>
-    <t>Dr. Monica Mahajan</t>
+    <t>Dr. Ramesh D</t>
+  </si>
+  <si>
+    <t>31 years experience overall</t>
+  </si>
+  <si>
+    <t>Ashok Nagar,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Vikram P S J</t>
+  </si>
+  <si>
+    <t>Greams Road,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Balaji R</t>
+  </si>
+  <si>
+    <t>24 years experience overall</t>
+  </si>
+  <si>
+    <t>Thousand Lights,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Nitya Narayanan</t>
+  </si>
+  <si>
+    <t>29 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. Sudha Anantha Krishnan</t>
+  </si>
+  <si>
+    <t>27 years experience overall</t>
+  </si>
+  <si>
+    <t>Kilpauk,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Nazira Sadique</t>
+  </si>
+  <si>
+    <t>Gynecologist/Obstetrician</t>
+  </si>
+  <si>
+    <t>39 years experience overall</t>
+  </si>
+  <si>
+    <t>Anna Nagar,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. P. V. Anuradha</t>
+  </si>
+  <si>
+    <t>36 years experience overall</t>
+  </si>
+  <si>
+    <t>Anna Nagar East,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Srikala Prasad</t>
+  </si>
+  <si>
+    <t>33 years experience overall</t>
+  </si>
+  <si>
+    <t>Vanagaram,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Parimalam Ramanathan</t>
   </si>
   <si>
     <t>30 years experience overall</t>
   </si>
   <si>
-    <t>Dr. Rajinder Kumar Singal</t>
-  </si>
-  <si>
-    <t>42 years experience overall</t>
-  </si>
-  <si>
-    <t>Dr. Ramesh D</t>
-  </si>
-  <si>
-    <t>31 years experience overall</t>
-  </si>
-  <si>
-    <t>Ashok Nagar,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Vikram P S J</t>
-  </si>
-  <si>
-    <t>Greams Road,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Balaji R</t>
-  </si>
-  <si>
-    <t>24 years experience overall</t>
-  </si>
-  <si>
-    <t>Thousand Lights,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Nitya Narayanan</t>
-  </si>
-  <si>
-    <t>29 years experience overall</t>
-  </si>
-  <si>
-    <t>Dr. Sudha Anantha Krishnan</t>
-  </si>
-  <si>
-    <t>27 years experience overall</t>
-  </si>
-  <si>
-    <t>Kilpauk,Chennai</t>
+    <t>Perungudi,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. M.H. Abinaya</t>
+  </si>
+  <si>
+    <t>22 years experience overall</t>
+  </si>
+  <si>
+    <t>T Nagar,Chennai</t>
   </si>
 </sst>
 </file>
@@ -697,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B91469-8571-4092-82B9-F8438CFB366A}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -794,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -829,16 +757,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -846,16 +774,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -863,16 +791,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -880,16 +808,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -897,16 +825,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"Deleted js for demo"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -463,6 +463,39 @@
   </si>
   <si>
     <t>Malleswaram,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. S Sarangapani</t>
+  </si>
+  <si>
+    <t>Ayurveda</t>
+  </si>
+  <si>
+    <t>44 years experience overall</t>
+  </si>
+  <si>
+    <t>Erragadda,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. M. Narasimha</t>
+  </si>
+  <si>
+    <t>Ameerpet,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. C Narmada</t>
+  </si>
+  <si>
+    <t>Shaikpet,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Priti Thakre</t>
+  </si>
+  <si>
+    <t>Dr. Sunita Grace</t>
+  </si>
+  <si>
+    <t>Banjara Hills,Hyderabad</t>
   </si>
 </sst>
 </file>
@@ -970,16 +1003,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -987,16 +1020,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -1004,16 +1037,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>48</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -1021,16 +1054,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>138</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -1038,16 +1071,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"JS by method arguments"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="203">
   <si>
     <t>Name</t>
   </si>
@@ -496,6 +496,156 @@
   </si>
   <si>
     <t>Banjara Hills,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Mrunal Godse</t>
+  </si>
+  <si>
+    <t>16 years experience overall</t>
+  </si>
+  <si>
+    <t>Kharadi,Pune</t>
+  </si>
+  <si>
+    <t>Dr. Kaustubh Patil</t>
+  </si>
+  <si>
+    <t>Dr. Bhushan Jawale</t>
+  </si>
+  <si>
+    <t>Pimpri-Chinchwad,Pune</t>
+  </si>
+  <si>
+    <t>Dr. Hemant Patil</t>
+  </si>
+  <si>
+    <t>17 years experience overall</t>
+  </si>
+  <si>
+    <t>Pimple Saudagar,Pune</t>
+  </si>
+  <si>
+    <t>Dr. Vishu A.Gupta</t>
+  </si>
+  <si>
+    <t>Aundh,Pune</t>
+  </si>
+  <si>
+    <t>Dr. Sonali Khaire</t>
+  </si>
+  <si>
+    <t>Andheri West,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Nidha Khan</t>
+  </si>
+  <si>
+    <t>Dr. Jay N. Harde</t>
+  </si>
+  <si>
+    <t>32 years experience overall</t>
+  </si>
+  <si>
+    <t>Borivali,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Zeba Radhanpura</t>
+  </si>
+  <si>
+    <t>11 years experience overall</t>
+  </si>
+  <si>
+    <t>Bandra West,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Shruti Sheth</t>
+  </si>
+  <si>
+    <t>Ghatkopar East,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Vinita Das</t>
+  </si>
+  <si>
+    <t>Dr. Sunita Chandra</t>
+  </si>
+  <si>
+    <t>Rajendranagar,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Smita Dwivedi</t>
+  </si>
+  <si>
+    <t>Charbagh,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Sonia Luthra</t>
+  </si>
+  <si>
+    <t>Lalbagh,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Swati Gautam</t>
+  </si>
+  <si>
+    <t>L D A Colony,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Sunil Yadav</t>
+  </si>
+  <si>
+    <t>Jankipuram,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Dipti Jain Bhalla</t>
+  </si>
+  <si>
+    <t>Chowk,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Mohammad Imran Khan</t>
+  </si>
+  <si>
+    <t>Daliganj,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Samarjit Singh</t>
+  </si>
+  <si>
+    <t>Telibagh,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Faiz Warsi</t>
+  </si>
+  <si>
+    <t>Vrindavan Colony,Lucknow</t>
+  </si>
+  <si>
+    <t>Dr. Venu Kumari</t>
+  </si>
+  <si>
+    <t>Dermatologist</t>
+  </si>
+  <si>
+    <t>Chanda Nagar,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Ravi Chandra V</t>
+  </si>
+  <si>
+    <t>AS Rao Nagar,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. D Subhash Reddy</t>
+  </si>
+  <si>
+    <t>Habsiguda,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Satyanarayana Murthy Komakula</t>
+  </si>
+  <si>
+    <t>Dr. B Anand</t>
   </si>
 </sst>
 </file>
@@ -1003,16 +1153,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>142</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>145</v>
+        <v>196</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -1020,16 +1170,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>146</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>147</v>
+        <v>198</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -1037,16 +1187,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>148</v>
+        <v>199</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>149</v>
+        <v>200</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -1054,16 +1204,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -1071,16 +1221,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>151</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"JS in methods for Demo"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="244">
   <si>
     <t>Name</t>
   </si>
@@ -646,6 +646,129 @@
   </si>
   <si>
     <t>Dr. B Anand</t>
+  </si>
+  <si>
+    <t>Dr. S C Rajendran</t>
+  </si>
+  <si>
+    <t>45 years experience overall</t>
+  </si>
+  <si>
+    <t>Koramangala,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Surendra V H H</t>
+  </si>
+  <si>
+    <t>43 years experience overall</t>
+  </si>
+  <si>
+    <t>Jayanagar,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. P S Murthy</t>
+  </si>
+  <si>
+    <t>42 years experience overall</t>
+  </si>
+  <si>
+    <t>Whitefield,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Mukesh Ramnane</t>
+  </si>
+  <si>
+    <t>41 years experience overall</t>
+  </si>
+  <si>
+    <t>Old Airport Road,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Shankar D Desai</t>
+  </si>
+  <si>
+    <t>Yeshwanthpur,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Dhershana Raja</t>
+  </si>
+  <si>
+    <t>Sarjapur Road,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Mukta Nadig</t>
+  </si>
+  <si>
+    <t>Sahakaranagar,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Sudhamathy Kannan</t>
+  </si>
+  <si>
+    <t>Dr. Deepak V Rao</t>
+  </si>
+  <si>
+    <t>37 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. T. M Jyothi Lakshmi</t>
+  </si>
+  <si>
+    <t>Dr. Aparna Singhal</t>
+  </si>
+  <si>
+    <t>Punjabi Bagh,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Ruchi Gupta</t>
+  </si>
+  <si>
+    <t>Pitampura,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Sanneya Manchanda</t>
+  </si>
+  <si>
+    <t>Jangpura,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Shivani Kataria</t>
+  </si>
+  <si>
+    <t>Patel Nagar West,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Shivani Mangal</t>
+  </si>
+  <si>
+    <t>Dwarka Sector 23,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Karishma Bhatia</t>
+  </si>
+  <si>
+    <t>Rohini,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Preeti Tahilyani</t>
+  </si>
+  <si>
+    <t>Dwarka,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Tejashri Shrotri</t>
+  </si>
+  <si>
+    <t>Hauz Khas,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Shalini Chaudhry</t>
+  </si>
+  <si>
+    <t>Dr. Shakuntla Shukla</t>
+  </si>
+  <si>
+    <t>Lajpat Nagar,Delhi</t>
   </si>
 </sst>
 </file>
@@ -1153,16 +1276,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>194</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>196</v>
+        <v>236</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -1170,16 +1293,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>69</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -1187,16 +1310,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>199</v>
+        <v>239</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -1204,16 +1327,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>138</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>198</v>
+        <v>238</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -1221,16 +1344,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>95</v>
+        <v>213</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>200</v>
+        <v>243</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"Removed JS for some, so that it runs for eclipse"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="262">
   <si>
     <t>Name</t>
   </si>
@@ -769,6 +769,60 @@
   </si>
   <si>
     <t>Lajpat Nagar,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Shambulingaiah S. Hiremath</t>
+  </si>
+  <si>
+    <t>Rajajinagar,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Chetali Samant</t>
+  </si>
+  <si>
+    <t>Dr. Shiny Menon</t>
+  </si>
+  <si>
+    <t>Dr. Chaya</t>
+  </si>
+  <si>
+    <t>Dr. Manjunath R Joshi</t>
+  </si>
+  <si>
+    <t>Bannerghatta Road,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Shantha Rama Rao</t>
+  </si>
+  <si>
+    <t>51 years experience overall</t>
+  </si>
+  <si>
+    <t>Kodambakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Bobby M</t>
+  </si>
+  <si>
+    <t>Thoraipakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Sathya Balasubramanyam</t>
+  </si>
+  <si>
+    <t>28 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. V. Bharathi</t>
+  </si>
+  <si>
+    <t>Mandaveli,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Karthiga Devi</t>
+  </si>
+  <si>
+    <t>Karapakkam,Chennai</t>
   </si>
 </sst>
 </file>
@@ -1276,16 +1330,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>40</v>
+        <v>252</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -1293,7 +1347,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>56</v>
@@ -1302,7 +1356,7 @@
         <v>69</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>238</v>
+        <v>255</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -1310,16 +1364,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>90</v>
+        <v>257</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>240</v>
+        <v>70</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -1327,16 +1381,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>238</v>
+        <v>259</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -1344,16 +1398,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="B6" t="s" s="0">
         <v>56</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>213</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>243</v>
+        <v>261</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"Changed the base class and hooks"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="298">
   <si>
     <t>Name</t>
   </si>
@@ -823,6 +823,114 @@
   </si>
   <si>
     <t>Karapakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Savita K</t>
+  </si>
+  <si>
+    <t>Banashankari 1st Stage,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Zadika Saeed P S</t>
+  </si>
+  <si>
+    <t>Jayanagar 9 Block,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Vishwaraj N</t>
+  </si>
+  <si>
+    <t>Seshadripuram,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Rita Samuel Bing</t>
+  </si>
+  <si>
+    <t>Kumaraswamy Layout,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Rakesh</t>
+  </si>
+  <si>
+    <t>Dr. Abhishek Sharma</t>
+  </si>
+  <si>
+    <t>South Extension 1,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Navjot Singh Arora</t>
+  </si>
+  <si>
+    <t>Dwarka Sector 6,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Sooneita Wagh Markan</t>
+  </si>
+  <si>
+    <t>34 years experience overall</t>
+  </si>
+  <si>
+    <t>Hari Nagar,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Ridhima Yadava</t>
+  </si>
+  <si>
+    <t>Dr. Pranay Kumar Agarwal</t>
+  </si>
+  <si>
+    <t>Park Circus,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Sudipta Chandra</t>
+  </si>
+  <si>
+    <t>Minto Park,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Sayan Ganguly</t>
+  </si>
+  <si>
+    <t>Dr. Sunil Jalan</t>
+  </si>
+  <si>
+    <t>Sarat Bose Road,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Nitin Mittal</t>
+  </si>
+  <si>
+    <t>Lake Town,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Vikram Deshmukh</t>
+  </si>
+  <si>
+    <t>Nanded City,Pune</t>
+  </si>
+  <si>
+    <t>Dr. Gautami Phadke</t>
+  </si>
+  <si>
+    <t>Karve Nagar,Pune</t>
+  </si>
+  <si>
+    <t>Dr. Nisha R. Patil</t>
+  </si>
+  <si>
+    <t>Dhanori,Pune</t>
+  </si>
+  <si>
+    <t>Dr. Abhinav Misuriya</t>
+  </si>
+  <si>
+    <t>Hadapsar,Pune</t>
+  </si>
+  <si>
+    <t>Dr. Ritesh Khandelwal</t>
+  </si>
+  <si>
+    <t>Lonavala,Pune</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1401,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -1324,22 +1432,19 @@
       <c r="E1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F1" t="s" s="0">
-        <v>32</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>251</v>
+        <v>288</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>252</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>253</v>
+        <v>289</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -1347,16 +1452,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>254</v>
+        <v>290</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>255</v>
+        <v>291</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -1364,16 +1469,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>256</v>
+        <v>292</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>257</v>
+        <v>92</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>70</v>
+        <v>293</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -1381,16 +1486,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>258</v>
+        <v>294</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>259</v>
+        <v>295</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -1398,16 +1503,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>261</v>
+        <v>297</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"Final Build, with & w/o JSE, added Screenshots, deleted comments"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2318520\eclipse-workspace\Hackathon_Practo\testFiles\"/>
     </mc:Choice>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -196,12 +196,139 @@
   </si>
   <si>
     <t>789JH982</t>
+  </si>
+  <si>
+    <t>Dr. N. Rajasekharam</t>
+  </si>
+  <si>
+    <t>Ear-Nose-Throat (ENT) Specialist</t>
+  </si>
+  <si>
+    <t>Ameerpet,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. S Neelima</t>
+  </si>
+  <si>
+    <t>14 years experience overall</t>
+  </si>
+  <si>
+    <t>Miyapur,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Krishna Bojja</t>
+  </si>
+  <si>
+    <t>21 years experience overall</t>
+  </si>
+  <si>
+    <t>Chanda Nagar,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. S.Nishanth</t>
+  </si>
+  <si>
+    <t>12 years experience overall</t>
+  </si>
+  <si>
+    <t>Pragathi Nagar,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. P.Ramakrishnaiah</t>
+  </si>
+  <si>
+    <t>Attapur,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Manohar K N</t>
+  </si>
+  <si>
+    <t>Internal Medicine</t>
+  </si>
+  <si>
+    <t>Old Airport Road,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Umesh Gupta</t>
+  </si>
+  <si>
+    <t>24 years experience overall</t>
+  </si>
+  <si>
+    <t>Hebbal,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Chhavi Goyal Mehra</t>
+  </si>
+  <si>
+    <t>General Physician</t>
+  </si>
+  <si>
+    <t>28 years experience overall</t>
+  </si>
+  <si>
+    <t>HSR Layout,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Prabha Ramadorai</t>
+  </si>
+  <si>
+    <t>26 years experience overall</t>
+  </si>
+  <si>
+    <t>Hulimavu,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Jai Babu</t>
+  </si>
+  <si>
+    <t>Cardiologist</t>
+  </si>
+  <si>
+    <t>HBR Layout,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Pranay Kumar Agarwal</t>
+  </si>
+  <si>
+    <t>13 years experience overall</t>
+  </si>
+  <si>
+    <t>Park Circus,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Sudipta Chandra</t>
+  </si>
+  <si>
+    <t>Minto Park,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Sayan Ganguly</t>
+  </si>
+  <si>
+    <t>31 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. Sunil Jalan</t>
+  </si>
+  <si>
+    <t>Sarat Bose Road,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Nitin Mittal</t>
+  </si>
+  <si>
+    <t>18 years experience overall</t>
+  </si>
+  <si>
+    <t>Lake Town,Kolkata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -576,11 +703,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.21875"/>
+    <col min="3" max="3" customWidth="true" width="16.21875"/>
+    <col min="4" max="4" customWidth="true" width="16.88671875"/>
+    <col min="5" max="5" customWidth="true" width="14.21875"/>
+    <col min="6" max="6" customWidth="true" width="21.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -604,10 +731,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -616,7 +743,7 @@
       <c r="D2" s="3">
         <v>6000000000</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -641,7 +768,7 @@
       <c r="D4" s="3">
         <v>9999999998</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>36</v>
       </c>
     </row>
@@ -649,7 +776,7 @@
       <c r="D5" s="3">
         <v>9999999999</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>7</v>
       </c>
     </row>
@@ -673,182 +800,182 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.5546875"/>
+    <col min="2" max="2" customWidth="true" width="27.44140625"/>
+    <col min="3" max="3" customWidth="true" width="24.109375"/>
+    <col min="4" max="4" customWidth="true" width="29.6640625"/>
+    <col min="5" max="5" customWidth="true" width="23.0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s" s="0">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s" s="0">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>90</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s" s="0">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s" s="0">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s" s="0">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E7" t="s">
+    <row r="7">
+      <c r="E7" t="s" s="0">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E8" t="s">
+    <row r="8">
+      <c r="E8" t="s" s="0">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
+    <row r="9">
+      <c r="E9" t="s" s="0">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E10" t="s">
+    <row r="10">
+      <c r="E10" t="s" s="0">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E11" t="s">
+    <row r="11">
+      <c r="E11" t="s" s="0">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E12" t="s">
+    <row r="12">
+      <c r="E12" t="s" s="0">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E13" t="s">
+    <row r="13">
+      <c r="E13" t="s" s="0">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E14" t="s">
+    <row r="14">
+      <c r="E14" t="s" s="0">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E15" t="s">
+    <row r="15">
+      <c r="E15" t="s" s="0">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="E16" t="s">
+    <row r="16">
+      <c r="E16" t="s" s="0">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" t="s">
+    <row r="17">
+      <c r="E17" t="s" s="0">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" t="s">
+    <row r="18">
+      <c r="E18" t="s" s="0">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
+    <row r="19">
+      <c r="E19" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E20" t="s">
+    <row r="20">
+      <c r="E20" t="s" s="0">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Final build w/o comments"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2318520\eclipse-workspace\Hackathon_Practo\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6DCF87-6F3C-42D9-B721-B6F1DC1447C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79DB88A-CEBB-4C47-8F76-BF91F5E045FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="708" windowWidth="23040" windowHeight="11532" xr2:uid="{CCA4E1CD-FF9D-4CD4-B2D1-E3BACCC0835E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="144">
   <si>
     <t>Name</t>
   </si>
@@ -156,46 +156,208 @@
     <t>22 years experience overall</t>
   </si>
   <si>
-    <t>Dr. Devisetty</t>
+    <t>789JH982</t>
+  </si>
+  <si>
+    <t>12 years experience overall</t>
+  </si>
+  <si>
+    <t>26 years experience overall</t>
+  </si>
+  <si>
+    <t>Gynecologist/Obstetrician</t>
+  </si>
+  <si>
+    <t>17 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. Sunipa Chatterjee</t>
+  </si>
+  <si>
+    <t>Beliaghata,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Suchandra Mukhopadhyay</t>
+  </si>
+  <si>
+    <t>Salt Lake,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Sankar Das Mahapatra</t>
+  </si>
+  <si>
+    <t>34 years experience overall</t>
+  </si>
+  <si>
+    <t>Teghoria,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Ranjana Tibrewal</t>
+  </si>
+  <si>
+    <t>Lake Gardens,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Shyamal Kumar Debnath</t>
+  </si>
+  <si>
+    <t>Dhakuria,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Shantha Rama Rao</t>
+  </si>
+  <si>
+    <t>51 years experience overall</t>
+  </si>
+  <si>
+    <t>Kodambakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. V. Bharathi</t>
+  </si>
+  <si>
+    <t>Mandaveli,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Bobby M</t>
+  </si>
+  <si>
+    <t>Thoraipakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Sathya Balasubramanyam</t>
+  </si>
+  <si>
+    <t>28 years experience overall</t>
+  </si>
+  <si>
+    <t>T Nagar,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Karthiga Devi</t>
+  </si>
+  <si>
+    <t>19 years experience overall</t>
+  </si>
+  <si>
+    <t>Karapakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Nikita Parasrampuria</t>
+  </si>
+  <si>
+    <t>Dentist</t>
+  </si>
+  <si>
+    <t>11 years experience overall</t>
+  </si>
+  <si>
+    <t>Lake Town,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Akshay Khandelwal</t>
+  </si>
+  <si>
+    <t>8 years experience overall</t>
+  </si>
+  <si>
+    <t>Barabazar,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Ananya Mishra</t>
+  </si>
+  <si>
+    <t>Dr. Somik Bose</t>
+  </si>
+  <si>
+    <t>16 years experience overall</t>
+  </si>
+  <si>
+    <t>Bhawanipore,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Manish Jha</t>
+  </si>
+  <si>
+    <t>15 years experience overall</t>
+  </si>
+  <si>
+    <t>Gariahat,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Siddhi Dinesh Prabhu</t>
+  </si>
+  <si>
+    <t>14 years experience overall</t>
+  </si>
+  <si>
+    <t>Grant Road,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Vivian Varghese</t>
+  </si>
+  <si>
+    <t>13 years experience overall</t>
+  </si>
+  <si>
+    <t>Borivali West,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Charmi Mehta</t>
+  </si>
+  <si>
+    <t>Kandivali West,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Rajesh Rajan</t>
+  </si>
+  <si>
+    <t>21 years experience overall</t>
+  </si>
+  <si>
+    <t>Deonar,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Rajiv Rajan</t>
+  </si>
+  <si>
+    <t>25 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. Inderpreet Batra</t>
   </si>
   <si>
     <t>Homoeopath</t>
   </si>
   <si>
-    <t>25 years experience overall</t>
-  </si>
-  <si>
-    <t>Senapati Bapat Marg,Pune</t>
-  </si>
-  <si>
-    <t>Dr. Hetal Vyas</t>
-  </si>
-  <si>
-    <t>Viman Nagar,Pune</t>
-  </si>
-  <si>
-    <t>Dr. Apeksha Devisetty</t>
-  </si>
-  <si>
-    <t>20 years experience overall</t>
-  </si>
-  <si>
-    <t>16 years experience overall</t>
-  </si>
-  <si>
-    <t>Pimpri-Chinchwad,Pune</t>
-  </si>
-  <si>
-    <t>Dr. Trupti Siddhesh Gurav</t>
-  </si>
-  <si>
-    <t>Dr. Deepanshu Thakur</t>
-  </si>
-  <si>
-    <t>Kalyani Nagar,Pune</t>
-  </si>
-  <si>
-    <t>789JH982</t>
+    <t>35 years experience overall</t>
+  </si>
+  <si>
+    <t>Greater Kailash Part 1,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Rupinder Kaur</t>
+  </si>
+  <si>
+    <t>Old Rajendra Nagar,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Gurpreet Juneja</t>
+  </si>
+  <si>
+    <t>Patel Nagar,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Ajay Kumar Grover</t>
+  </si>
+  <si>
+    <t>33 years experience overall</t>
+  </si>
+  <si>
+    <t>Dr. Shweta Bhandari</t>
+  </si>
+  <si>
+    <t>Krishna Nagar,Delhi</t>
   </si>
   <si>
     <t>Dr. N. Rajasekharam</t>
@@ -210,28 +372,19 @@
     <t>Dr. S Neelima</t>
   </si>
   <si>
-    <t>14 years experience overall</t>
-  </si>
-  <si>
     <t>Miyapur,Hyderabad</t>
   </si>
   <si>
     <t>Dr. Krishna Bojja</t>
   </si>
   <si>
-    <t>21 years experience overall</t>
-  </si>
-  <si>
     <t>Chanda Nagar,Hyderabad</t>
   </si>
   <si>
     <t>Dr. S.Nishanth</t>
   </si>
   <si>
-    <t>12 years experience overall</t>
-  </si>
-  <si>
-    <t>Pragathi Nagar,Hyderabad</t>
+    <t>Nacharam,Hyderabad</t>
   </si>
   <si>
     <t>Dr. P.Ramakrishnaiah</t>
@@ -240,88 +393,82 @@
     <t>Attapur,Hyderabad</t>
   </si>
   <si>
-    <t>Dr. Manohar K N</t>
-  </si>
-  <si>
-    <t>Internal Medicine</t>
-  </si>
-  <si>
-    <t>Old Airport Road,Bangalore</t>
-  </si>
-  <si>
-    <t>Dr. Umesh Gupta</t>
-  </si>
-  <si>
-    <t>24 years experience overall</t>
-  </si>
-  <si>
-    <t>Hebbal,Bangalore</t>
-  </si>
-  <si>
-    <t>Dr. Chhavi Goyal Mehra</t>
-  </si>
-  <si>
-    <t>General Physician</t>
-  </si>
-  <si>
-    <t>28 years experience overall</t>
-  </si>
-  <si>
-    <t>HSR Layout,Bangalore</t>
-  </si>
-  <si>
-    <t>Dr. Prabha Ramadorai</t>
-  </si>
-  <si>
-    <t>26 years experience overall</t>
-  </si>
-  <si>
-    <t>Hulimavu,Bangalore</t>
-  </si>
-  <si>
-    <t>Dr. Jai Babu</t>
-  </si>
-  <si>
-    <t>Cardiologist</t>
-  </si>
-  <si>
-    <t>HBR Layout,Bangalore</t>
-  </si>
-  <si>
-    <t>Dr. Pranay Kumar Agarwal</t>
-  </si>
-  <si>
-    <t>13 years experience overall</t>
-  </si>
-  <si>
-    <t>Park Circus,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Sudipta Chandra</t>
-  </si>
-  <si>
-    <t>Minto Park,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Sayan Ganguly</t>
-  </si>
-  <si>
-    <t>31 years experience overall</t>
-  </si>
-  <si>
-    <t>Dr. Sunil Jalan</t>
-  </si>
-  <si>
-    <t>Sarat Bose Road,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Nitin Mittal</t>
-  </si>
-  <si>
-    <t>18 years experience overall</t>
-  </si>
-  <si>
-    <t>Lake Town,Kolkata</t>
+    <t>Dr. Vijay Dagar</t>
+  </si>
+  <si>
+    <t>Ayurveda</t>
+  </si>
+  <si>
+    <t>Uttam Nagar,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Vishwa Deep Biswas</t>
+  </si>
+  <si>
+    <t>7 years experience overall</t>
+  </si>
+  <si>
+    <t>Punjabi Bagh,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Ruchi Gupta</t>
+  </si>
+  <si>
+    <t>23 years experience overall</t>
+  </si>
+  <si>
+    <t>Rohini,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Manju Singh</t>
+  </si>
+  <si>
+    <t>30 years experience overall</t>
+  </si>
+  <si>
+    <t>Connaught Place,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Shyla Vahab</t>
+  </si>
+  <si>
+    <t>Dwarka Sector 13,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Katheeja Nasika</t>
+  </si>
+  <si>
+    <t>Dermatologist</t>
+  </si>
+  <si>
+    <t>Chromepet,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Nithila M</t>
+  </si>
+  <si>
+    <t>Adyar,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Sai Preethi</t>
+  </si>
+  <si>
+    <t>9 years experience overall</t>
+  </si>
+  <si>
+    <t>Alwarpet,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Shraddha</t>
+  </si>
+  <si>
+    <t>Greams Road,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Sowmya Dogiparthi</t>
+  </si>
+  <si>
+    <t>Thousand Lights,Chennai</t>
   </si>
 </sst>
 </file>
@@ -704,9 +851,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="14.21875"/>
-    <col min="3" max="3" customWidth="true" width="16.21875"/>
+    <col min="3" max="3" customWidth="true" width="17.109375"/>
     <col min="4" max="4" customWidth="true" width="16.88671875"/>
-    <col min="5" max="5" customWidth="true" width="14.21875"/>
+    <col min="5" max="5" customWidth="true" width="18.0"/>
     <col min="6" max="6" customWidth="true" width="21.6640625"/>
   </cols>
   <sheetData>
@@ -738,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3">
         <v>6000000000</v>
@@ -800,9 +947,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.5546875"/>
+    <col min="1" max="1" customWidth="true" width="31.21875"/>
     <col min="2" max="2" customWidth="true" width="27.44140625"/>
-    <col min="3" max="3" customWidth="true" width="24.109375"/>
+    <col min="3" max="3" customWidth="true" width="27.0"/>
     <col min="4" max="4" customWidth="true" width="29.6640625"/>
     <col min="5" max="5" customWidth="true" width="23.0"/>
   </cols>
@@ -826,16 +973,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -843,16 +990,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>86</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -860,16 +1007,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>89</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -877,16 +1024,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>91</v>
+        <v>141</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -894,16 +1041,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>54</v>
+        <v>133</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"Final Build with tags, comments, Logs, ScreenShots, Reports"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2318520\eclipse-workspace\Hackathon_Practo\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79DB88A-CEBB-4C47-8F76-BF91F5E045FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20653A3-EB44-4FD8-8159-96CF7F6751F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="708" windowWidth="23040" windowHeight="11532" xr2:uid="{CCA4E1CD-FF9D-4CD4-B2D1-E3BACCC0835E}"/>
+    <workbookView xWindow="0" yWindow="708" windowWidth="23040" windowHeight="11532" activeTab="1" xr2:uid="{CCA4E1CD-FF9D-4CD4-B2D1-E3BACCC0835E}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -159,323 +159,46 @@
     <t>789JH982</t>
   </si>
   <si>
-    <t>12 years experience overall</t>
-  </si>
-  <si>
     <t>26 years experience overall</t>
   </si>
   <si>
-    <t>Gynecologist/Obstetrician</t>
-  </si>
-  <si>
-    <t>17 years experience overall</t>
-  </si>
-  <si>
-    <t>Dr. Sunipa Chatterjee</t>
-  </si>
-  <si>
-    <t>Beliaghata,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Suchandra Mukhopadhyay</t>
-  </si>
-  <si>
-    <t>Salt Lake,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Sankar Das Mahapatra</t>
-  </si>
-  <si>
-    <t>34 years experience overall</t>
-  </si>
-  <si>
-    <t>Teghoria,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Ranjana Tibrewal</t>
-  </si>
-  <si>
-    <t>Lake Gardens,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Shyamal Kumar Debnath</t>
-  </si>
-  <si>
-    <t>Dhakuria,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Shantha Rama Rao</t>
-  </si>
-  <si>
-    <t>51 years experience overall</t>
-  </si>
-  <si>
-    <t>Kodambakkam,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. V. Bharathi</t>
-  </si>
-  <si>
-    <t>Mandaveli,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Bobby M</t>
-  </si>
-  <si>
-    <t>Thoraipakkam,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Sathya Balasubramanyam</t>
-  </si>
-  <si>
     <t>28 years experience overall</t>
   </si>
   <si>
-    <t>T Nagar,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Karthiga Devi</t>
-  </si>
-  <si>
-    <t>19 years experience overall</t>
-  </si>
-  <si>
-    <t>Karapakkam,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Nikita Parasrampuria</t>
-  </si>
-  <si>
-    <t>Dentist</t>
-  </si>
-  <si>
-    <t>11 years experience overall</t>
-  </si>
-  <si>
-    <t>Lake Town,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Akshay Khandelwal</t>
-  </si>
-  <si>
-    <t>8 years experience overall</t>
-  </si>
-  <si>
-    <t>Barabazar,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Ananya Mishra</t>
-  </si>
-  <si>
-    <t>Dr. Somik Bose</t>
-  </si>
-  <si>
     <t>16 years experience overall</t>
   </si>
   <si>
-    <t>Bhawanipore,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Manish Jha</t>
-  </si>
-  <si>
-    <t>15 years experience overall</t>
-  </si>
-  <si>
-    <t>Gariahat,Kolkata</t>
-  </si>
-  <si>
-    <t>Dr. Siddhi Dinesh Prabhu</t>
-  </si>
-  <si>
-    <t>14 years experience overall</t>
-  </si>
-  <si>
-    <t>Grant Road,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Vivian Varghese</t>
-  </si>
-  <si>
     <t>13 years experience overall</t>
   </si>
   <si>
-    <t>Borivali West,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Charmi Mehta</t>
-  </si>
-  <si>
-    <t>Kandivali West,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Rajesh Rajan</t>
-  </si>
-  <si>
-    <t>21 years experience overall</t>
-  </si>
-  <si>
-    <t>Deonar,Mumbai</t>
-  </si>
-  <si>
-    <t>Dr. Rajiv Rajan</t>
-  </si>
-  <si>
-    <t>25 years experience overall</t>
-  </si>
-  <si>
-    <t>Dr. Inderpreet Batra</t>
-  </si>
-  <si>
-    <t>Homoeopath</t>
-  </si>
-  <si>
-    <t>35 years experience overall</t>
-  </si>
-  <si>
-    <t>Greater Kailash Part 1,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Rupinder Kaur</t>
-  </si>
-  <si>
-    <t>Old Rajendra Nagar,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Gurpreet Juneja</t>
-  </si>
-  <si>
-    <t>Patel Nagar,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Ajay Kumar Grover</t>
-  </si>
-  <si>
-    <t>33 years experience overall</t>
-  </si>
-  <si>
-    <t>Dr. Shweta Bhandari</t>
-  </si>
-  <si>
-    <t>Krishna Nagar,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. N. Rajasekharam</t>
-  </si>
-  <si>
-    <t>Ear-Nose-Throat (ENT) Specialist</t>
-  </si>
-  <si>
-    <t>Ameerpet,Hyderabad</t>
-  </si>
-  <si>
-    <t>Dr. S Neelima</t>
-  </si>
-  <si>
-    <t>Miyapur,Hyderabad</t>
-  </si>
-  <si>
-    <t>Dr. Krishna Bojja</t>
-  </si>
-  <si>
-    <t>Chanda Nagar,Hyderabad</t>
-  </si>
-  <si>
-    <t>Dr. S.Nishanth</t>
-  </si>
-  <si>
-    <t>Nacharam,Hyderabad</t>
-  </si>
-  <si>
-    <t>Dr. P.Ramakrishnaiah</t>
-  </si>
-  <si>
-    <t>Attapur,Hyderabad</t>
-  </si>
-  <si>
-    <t>Dr. Vijay Dagar</t>
-  </si>
-  <si>
     <t>Ayurveda</t>
   </si>
   <si>
-    <t>Uttam Nagar,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Vishwa Deep Biswas</t>
-  </si>
-  <si>
-    <t>7 years experience overall</t>
-  </si>
-  <si>
-    <t>Punjabi Bagh,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Ruchi Gupta</t>
-  </si>
-  <si>
-    <t>23 years experience overall</t>
-  </si>
-  <si>
-    <t>Rohini,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Manju Singh</t>
-  </si>
-  <si>
-    <t>30 years experience overall</t>
-  </si>
-  <si>
-    <t>Connaught Place,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Shyla Vahab</t>
-  </si>
-  <si>
-    <t>Dwarka Sector 13,Delhi</t>
-  </si>
-  <si>
-    <t>Dr. Katheeja Nasika</t>
-  </si>
-  <si>
-    <t>Dermatologist</t>
-  </si>
-  <si>
-    <t>Chromepet,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Nithila M</t>
-  </si>
-  <si>
-    <t>Adyar,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Sai Preethi</t>
-  </si>
-  <si>
-    <t>9 years experience overall</t>
-  </si>
-  <si>
-    <t>Alwarpet,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Shraddha</t>
-  </si>
-  <si>
-    <t>Greams Road,Chennai</t>
-  </si>
-  <si>
-    <t>Dr. Sowmya Dogiparthi</t>
-  </si>
-  <si>
-    <t>Thousand Lights,Chennai</t>
+    <t>Dr. Uday Kiran</t>
+  </si>
+  <si>
+    <t>West Mambalam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. T. Vamsi Latha</t>
+  </si>
+  <si>
+    <t>Dr. Sampoorna M</t>
+  </si>
+  <si>
+    <t>Dr. Poonam Verma</t>
+  </si>
+  <si>
+    <t>Vadapalani,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. D Srikrishna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -844,17 +567,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B91469-8571-4092-82B9-F8438CFB366A}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="14.21875"/>
-    <col min="3" max="3" customWidth="true" width="17.109375"/>
-    <col min="4" max="4" customWidth="true" width="16.88671875"/>
-    <col min="5" max="5" customWidth="true" width="18.0"/>
-    <col min="6" max="6" customWidth="true" width="21.6640625"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -878,10 +601,10 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -890,7 +613,7 @@
       <c r="D2" s="3">
         <v>6000000000</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>33</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -915,7 +638,7 @@
       <c r="D4" s="3">
         <v>9999999998</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -923,7 +646,7 @@
       <c r="D5" s="3">
         <v>9999999999</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -941,188 +664,188 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.21875"/>
-    <col min="2" max="2" customWidth="true" width="27.44140625"/>
-    <col min="3" max="3" customWidth="true" width="27.0"/>
-    <col min="4" max="4" customWidth="true" width="29.6640625"/>
-    <col min="5" max="5" customWidth="true" width="23.0"/>
+    <col min="1" max="1" width="31.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>132</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>134</v>
-      </c>
-      <c r="E2" t="s" s="0">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>135</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>122</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>136</v>
-      </c>
-      <c r="E3" t="s" s="0">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>137</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>138</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>139</v>
-      </c>
-      <c r="E4" t="s" s="0">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>140</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>141</v>
-      </c>
-      <c r="E5" t="s" s="0">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>142</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>133</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>80</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>143</v>
-      </c>
-      <c r="E6" t="s" s="0">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7">
-      <c r="E7" t="s" s="0">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8">
-      <c r="E8" t="s" s="0">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9">
-      <c r="E9" t="s" s="0">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10">
-      <c r="E10" t="s" s="0">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11">
-      <c r="E11" t="s" s="0">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12">
-      <c r="E12" t="s" s="0">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13">
-      <c r="E13" t="s" s="0">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14">
-      <c r="E14" t="s" s="0">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15">
-      <c r="E15" t="s" s="0">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16">
-      <c r="E16" t="s" s="0">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17">
-      <c r="E17" t="s" s="0">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18">
-      <c r="E18" t="s" s="0">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19">
-      <c r="E19" t="s" s="0">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20">
-      <c r="E20" t="s" s="0">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Final changes, with exception handling"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="182">
   <si>
     <t>Name</t>
   </si>
@@ -349,6 +349,240 @@
   </si>
   <si>
     <t>Defence Colony,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Sandhya</t>
+  </si>
+  <si>
+    <t>Homoeopath</t>
+  </si>
+  <si>
+    <t>Manikonda,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Vidya Lakshmi I</t>
+  </si>
+  <si>
+    <t>Sanath Nagar,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. RamaKrishna</t>
+  </si>
+  <si>
+    <t>Dilsukhnagar,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Subhash Chander</t>
+  </si>
+  <si>
+    <t>52 years experience overall</t>
+  </si>
+  <si>
+    <t>Jeedimetla,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Seshasaina Reddy</t>
+  </si>
+  <si>
+    <t>23 years experience overall</t>
+  </si>
+  <si>
+    <t>Madhapur,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Jayant Thakuria</t>
+  </si>
+  <si>
+    <t>Internal Medicine</t>
+  </si>
+  <si>
+    <t>25 years experience overall</t>
+  </si>
+  <si>
+    <t>East Of Kailash,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Monica Mahajan</t>
+  </si>
+  <si>
+    <t>30 years experience overall</t>
+  </si>
+  <si>
+    <t>Saket,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Anil Vardani</t>
+  </si>
+  <si>
+    <t>38 years experience overall</t>
+  </si>
+  <si>
+    <t>Pusa Road,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Yogesh Kumar Chhabra</t>
+  </si>
+  <si>
+    <t>Nephrologist</t>
+  </si>
+  <si>
+    <t>Shalimar Bagh,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. Mukesh Mehra</t>
+  </si>
+  <si>
+    <t>40 years experience overall</t>
+  </si>
+  <si>
+    <t>Patparganj,Delhi</t>
+  </si>
+  <si>
+    <t>Dr. N. Rajasekharam</t>
+  </si>
+  <si>
+    <t>Ear-Nose-Throat (ENT) Specialist</t>
+  </si>
+  <si>
+    <t>Ameerpet,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. S Neelima</t>
+  </si>
+  <si>
+    <t>Miyapur,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Krishna Bojja</t>
+  </si>
+  <si>
+    <t>Chanda Nagar,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. S.Nishanth</t>
+  </si>
+  <si>
+    <t>Nacharam,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. P.Ramakrishnaiah</t>
+  </si>
+  <si>
+    <t>Attapur,Hyderabad</t>
+  </si>
+  <si>
+    <t>Dr. Latha Shankar</t>
+  </si>
+  <si>
+    <t>Sahakaranagar,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Triveni</t>
+  </si>
+  <si>
+    <t>Hebbal,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Achi Ashok</t>
+  </si>
+  <si>
+    <t>HSR Layout,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Aruna Kumari V</t>
+  </si>
+  <si>
+    <t>Bellandur,Bangalore</t>
+  </si>
+  <si>
+    <t>Yelahanka,Bangalore</t>
+  </si>
+  <si>
+    <t>Dr. Shantha Rama Rao</t>
+  </si>
+  <si>
+    <t>51 years experience overall</t>
+  </si>
+  <si>
+    <t>Kodambakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Bobby M</t>
+  </si>
+  <si>
+    <t>Thoraipakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Sathya Balasubramanyam</t>
+  </si>
+  <si>
+    <t>T Nagar,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. V. Bharathi</t>
+  </si>
+  <si>
+    <t>Mandaveli,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Karthiga Devi</t>
+  </si>
+  <si>
+    <t>Karapakkam,Chennai</t>
+  </si>
+  <si>
+    <t>Dr. Barnali Dutta</t>
+  </si>
+  <si>
+    <t>Dermatologist</t>
+  </si>
+  <si>
+    <t>Jodhpur Park,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Nidhi jindal</t>
+  </si>
+  <si>
+    <t>Dr. Aarti Sarda</t>
+  </si>
+  <si>
+    <t>Dhakuria,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Reeja Mariam George</t>
+  </si>
+  <si>
+    <t>Dr. Priyanka Aggarwal</t>
+  </si>
+  <si>
+    <t>New Town,Kolkata</t>
+  </si>
+  <si>
+    <t>Dr. Kiran Katkar</t>
+  </si>
+  <si>
+    <t>Dadar West,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Sonia Tekchandani</t>
+  </si>
+  <si>
+    <t>Andheri West,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Jolly Shah Kapadia</t>
+  </si>
+  <si>
+    <t>Mulund West,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Resham Vasani Bhojani</t>
+  </si>
+  <si>
+    <t>Matunga,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Zeenat Bhalwani</t>
   </si>
 </sst>
 </file>
@@ -853,16 +1087,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>93</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>95</v>
+        <v>174</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -870,16 +1104,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>96</v>
+        <v>175</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -887,16 +1121,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>98</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>99</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -904,16 +1138,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>100</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>101</v>
+        <v>180</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -921,16 +1155,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>102</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>69</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>103</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>

<commit_message>
"Added JSE get text"
</commit_message>
<xml_diff>
--- a/testFiles/TestData.xlsx
+++ b/testFiles/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="213">
   <si>
     <t>Name</t>
   </si>
@@ -646,6 +646,36 @@
   </si>
   <si>
     <t>Dr. M.Srikanth</t>
+  </si>
+  <si>
+    <t>Dr. Divya Prabhat</t>
+  </si>
+  <si>
+    <t>Mahim,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Jaideep Mankani</t>
+  </si>
+  <si>
+    <t>33 years experience overall</t>
+  </si>
+  <si>
+    <t>Kandivali East,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Krishna Vora</t>
+  </si>
+  <si>
+    <t>Tardeo,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Sonali Pandit</t>
+  </si>
+  <si>
+    <t>Chembur,Mumbai</t>
+  </si>
+  <si>
+    <t>Dr. Ajay Doiphode</t>
   </si>
 </sst>
 </file>
@@ -1150,16 +1180,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>193</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>13</v>
@@ -1167,16 +1197,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>14</v>
@@ -1184,16 +1214,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>15</v>
@@ -1201,16 +1231,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="E5" t="s" s="0">
         <v>16</v>
@@ -1218,16 +1248,16 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="E6" t="s" s="0">
         <v>17</v>

</xml_diff>